<commit_message>
Se hizo la adecuación Clientes con VRUT
Se requiere introducir la function que calcula el Verificador del RUT
</commit_message>
<xml_diff>
--- a/1 - Documentos/Campos Solicitud de Despacho.xlsx
+++ b/1 - Documentos/Campos Solicitud de Despacho.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Mimet\MiLogistic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\David\Despacho\1 - Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F744BBE-90DB-4D92-A583-7FE53FF8B9F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{5AE6A2BE-3076-4028-A2E9-ADF351E88C07}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="Campos Formulario" sheetId="1" r:id="rId1"/>
@@ -270,7 +269,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,69 +320,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1BF1C5A3-F14F-44F9-806E-8161BA33C647}" name="Tabla2" displayName="Tabla2" ref="B2:H41" totalsRowShown="0">
-  <autoFilter ref="B2:H41" xr:uid="{5B287F3F-F715-43E5-A942-7CDE4A0DD7CF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="B2:H41" totalsRowShown="0">
+  <autoFilter ref="B2:H41"/>
   <sortState ref="B3:H41">
     <sortCondition ref="G2:G41"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{03747078-93C7-4D95-857A-AD1B3ED9D1B4}" name="NOMBRE CAMPO"/>
-    <tableColumn id="2" xr3:uid="{7B1131D4-F026-4224-8857-F2168F561BCA}" name="TIPO DATO"/>
-    <tableColumn id="6" xr3:uid="{FBBBEEA0-6105-4B68-90C2-2D28AC4CA76B}" name="ORIGEN"/>
-    <tableColumn id="7" xr3:uid="{4FBDA2DA-E1D2-4221-94FA-AE0FA71A4325}" name="FORMATO"/>
-    <tableColumn id="3" xr3:uid="{E39CE881-BBA1-4FF5-BB6C-52B3958AEF4F}" name="RESPONSABLE"/>
-    <tableColumn id="4" xr3:uid="{04982495-7A0B-4355-A325-8FED5B961008}" name="FASE FORMULARIO"/>
-    <tableColumn id="8" xr3:uid="{8D815C1F-CC66-4FEB-8CD7-ACB807CD1E84}" name="AUTOMÁTICO"/>
+    <tableColumn id="1" name="NOMBRE CAMPO"/>
+    <tableColumn id="2" name="TIPO DATO"/>
+    <tableColumn id="6" name="ORIGEN"/>
+    <tableColumn id="7" name="FORMATO"/>
+    <tableColumn id="3" name="RESPONSABLE"/>
+    <tableColumn id="4" name="FASE FORMULARIO"/>
+    <tableColumn id="8" name="AUTOMÁTICO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E233A0EB-8D06-4337-8009-53C99CCAEC28}" name="Tabla3" displayName="Tabla3" ref="B2:B10" totalsRowShown="0">
-  <autoFilter ref="B2:B10" xr:uid="{48AE1D27-E071-493B-AD84-A51989486DC7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="B2:B10" totalsRowShown="0">
+  <autoFilter ref="B2:B10"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{16029C63-7460-4E6C-86AB-793173F49E1F}" name="TIPOS DE DATO"/>
+    <tableColumn id="1" name="TIPOS DE DATO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B6AEE36-BB28-4361-8FA2-607049C78414}" name="Tabla1" displayName="Tabla1" ref="D2:D6" totalsRowShown="0">
-  <autoFilter ref="D2:D6" xr:uid="{F425EF29-F210-494B-A9DB-A8A5530675E0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="D2:D6" totalsRowShown="0">
+  <autoFilter ref="D2:D6"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C9B509A1-2EFE-4095-9BFE-E105168FDD5C}" name="ORIGEN"/>
+    <tableColumn id="1" name="ORIGEN"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3360F531-26F7-4E1E-9C01-09E14B0FDB88}" name="Tabla4" displayName="Tabla4" ref="F2:F10" totalsRowShown="0">
-  <autoFilter ref="F2:F10" xr:uid="{6B1AC7E5-DC57-4480-8B63-B15B27D8B6B0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="F2:F10" totalsRowShown="0">
+  <autoFilter ref="F2:F10"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{CFDBBA68-6011-4931-A10A-BE24D1E9E745}" name="FORMATO"/>
+    <tableColumn id="1" name="FORMATO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{11FBAD7C-DF65-494B-ACDF-21394107E1F7}" name="Tabla5" displayName="Tabla5" ref="H2:H5" totalsRowShown="0">
-  <autoFilter ref="H2:H5" xr:uid="{075681D2-4D10-4E68-A133-C9DCB89F699F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="H2:H5" totalsRowShown="0">
+  <autoFilter ref="H2:H5"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C0395228-C44F-4C5B-893F-132C2FB6F6DC}" name="RESPONSABLE"/>
+    <tableColumn id="1" name="RESPONSABLE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D7715EC1-06AD-4998-8E2B-35DA2F66D6E2}" name="Tabla6" displayName="Tabla6" ref="J2:J9" totalsRowShown="0">
-  <autoFilter ref="J2:J9" xr:uid="{FC411036-3D6F-4177-85D5-02EC7CF34DBF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="J2:J9" totalsRowShown="0">
+  <autoFilter ref="J2:J9"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1FD06791-8231-4A98-915B-05599F0842C8}" name="Fases"/>
+    <tableColumn id="1" name="Fases"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -685,25 +684,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CFCEE0-2810-443B-9F26-B9E99521FF49}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.2265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.31640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.31640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.76953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.76953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -726,7 +725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -749,7 +748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>28</v>
       </c>
@@ -772,7 +771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>29</v>
       </c>
@@ -795,7 +794,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -818,7 +817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>48</v>
       </c>
@@ -841,7 +840,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>49</v>
       </c>
@@ -864,7 +863,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>50</v>
       </c>
@@ -887,7 +886,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>51</v>
       </c>
@@ -910,7 +909,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>52</v>
       </c>
@@ -933,7 +932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>53</v>
       </c>
@@ -956,7 +955,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>54</v>
       </c>
@@ -979,7 +978,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>55</v>
       </c>
@@ -1002,7 +1001,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>57</v>
       </c>
@@ -1025,12 +1024,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -1048,7 +1047,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>59</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -1094,7 +1093,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>62</v>
       </c>
@@ -1117,7 +1116,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>63</v>
       </c>
@@ -1140,7 +1139,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>64</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -1186,7 +1185,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>66</v>
       </c>
@@ -1209,7 +1208,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>38</v>
       </c>
@@ -1232,7 +1231,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>35</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>36</v>
       </c>
@@ -1278,7 +1277,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>37</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>46</v>
       </c>
@@ -1324,7 +1323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>47</v>
       </c>
@@ -1347,7 +1346,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>73</v>
       </c>
@@ -1370,7 +1369,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>67</v>
       </c>
@@ -1393,7 +1392,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>68</v>
       </c>
@@ -1416,7 +1415,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>69</v>
       </c>
@@ -1439,7 +1438,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>70</v>
       </c>
@@ -1462,7 +1461,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>71</v>
       </c>
@@ -1485,7 +1484,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>72</v>
       </c>
@@ -1508,7 +1507,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>74</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>76</v>
       </c>
@@ -1554,7 +1553,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>14</v>
       </c>
@@ -1577,7 +1576,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>77</v>
       </c>
@@ -1600,7 +1599,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.75">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>45</v>
       </c>
@@ -1631,31 +1630,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9739B117-1797-4793-9E3E-2828E6F87800}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Utilidades!$B$3:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>C3:C41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D343225-FB85-428A-BB77-E1A64762AA2E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Utilidades!$H$3:$H$5</xm:f>
           </x14:formula1>
           <xm:sqref>F3:F41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A69579F8-B783-4399-966E-DB8343842AE5}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Utilidades!$J$3:$J$9</xm:f>
           </x14:formula1>
           <xm:sqref>G3:G41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E6B55717-7C6E-4F45-A963-852D976340C1}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Utilidades!$F$3:$F$10</xm:f>
           </x14:formula1>
           <xm:sqref>E3:E41</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B8E47B63-C8CF-4E93-86A2-7D1417C88998}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Utilidades!$D$3:$D$6</xm:f>
           </x14:formula1>
@@ -1668,23 +1667,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E208BB-622E-484F-95F6-863B5CF43AE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.76953125" customWidth="1"/>
-    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.31640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.76953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.75">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -1701,7 +1700,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -1735,7 +1734,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -1752,7 +1751,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -1766,7 +1765,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -1777,7 +1776,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -1788,7 +1787,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.75">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>60</v>
       </c>

</xml_diff>